<commit_message>
stat functions are now consistently ignore non-numeric values
</commit_message>
<xml_diff>
--- a/ACQ.Excel/ACQ.Stats.xlsx
+++ b/ACQ.Excel/ACQ.Stats.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C692BA0-16A0-42A1-9681-E97AD48B241A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E71F19D-08C8-45E5-9F6A-C67FDED8894D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3345" yWindow="1830" windowWidth="24450" windowHeight="12690" tabRatio="900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
     <sheet name="Stats" sheetId="21" r:id="rId2"/>
+    <sheet name="BinomialConfidence" sheetId="22" r:id="rId3"/>
+    <sheet name="MinMax" sheetId="23" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>date</t>
   </si>
@@ -150,6 +152,54 @@
   </si>
   <si>
     <t>weighted</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>confidance</t>
+  </si>
+  <si>
+    <t>acq_binomtest</t>
+  </si>
+  <si>
+    <t>acq_max</t>
+  </si>
+  <si>
+    <t>acq_absmax</t>
+  </si>
+  <si>
+    <t>acq_min</t>
+  </si>
+  <si>
+    <t>acq_abmin</t>
+  </si>
+  <si>
+    <t>acq_sum</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>ACQ</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>acq_stdev</t>
+  </si>
+  <si>
+    <t>acq_sumofsquares</t>
   </si>
 </sst>
 </file>
@@ -387,7 +437,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -412,6 +462,9 @@
     <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="5" fillId="4" borderId="2" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -786,18 +839,18 @@
       </c>
       <c r="C4" s="6" t="str">
         <f>_xll.acq_version()</f>
-        <v>1.3.8030.35923</v>
+        <v>1.4.8035.38349</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="13">
         <f ca="1">TODAY()</f>
-        <v>44556</v>
+        <v>44561</v>
       </c>
       <c r="J4" s="14" t="str">
         <f ca="1">_xll.acq_tostring(H4)</f>
-        <v>44556</v>
+        <v>44561</v>
       </c>
     </row>
     <row r="5" spans="2:10">
@@ -919,7 +972,7 @@
       </c>
       <c r="H13" t="str">
         <f ca="1">_xll.acq_join(H3:H10)</f>
-        <v>3.14159265358979,44556,True,,,,,</v>
+        <v>3.14159265358979,44561,True,,,,,</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" thickBot="1">
@@ -928,7 +981,7 @@
       </c>
       <c r="H14" t="str">
         <f ca="1">_xll.acq_join(J3:J10, "|")</f>
-        <v>3.14159265358979|44556|TRUE|||||</v>
+        <v>3.14159265358979|44561|TRUE|||||</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1">
@@ -1475,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3652BA-B6C4-41DD-BA87-7F24132F99FF}">
   <dimension ref="A3:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1844,4 +1897,829 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F123368-5BB9-4931-95EC-690D8D570C5B}">
+  <dimension ref="A2:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="E5">
+        <v>-1</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5" t="e">
+        <f>_xll.acq_binomtest(E5,F5,$B$2,TRUE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H5" t="e">
+        <f>_xll.acq_binomtest(E5,F5,$B$2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <f>_xll.acq_binomtest(E6,F6,$B$2,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f>_xll.acq_binomtest(E6,F6,$B$2,FALSE)</f>
+        <v>0.2775327998628892</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <f>_xll.acq_binomtest(E7,F7,$B$2,TRUE)</f>
+        <v>1.7876213095072889E-2</v>
+      </c>
+      <c r="H7">
+        <f>_xll.acq_binomtest(E7,F7,$B$2,FALSE)</f>
+        <v>0.40415002679523848</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <f>_xll.acq_binomtest(E8,F8,$B$2,TRUE)</f>
+        <v>5.6682151454375218E-2</v>
+      </c>
+      <c r="H8">
+        <f>_xll.acq_binomtest(E8,F8,$B$2,FALSE)</f>
+        <v>0.50983752846335817</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <f>_xll.acq_binomtest(E9,F9,$B$2,TRUE)</f>
+        <v>0.10779126740630099</v>
+      </c>
+      <c r="H9">
+        <f>_xll.acq_binomtest(E9,F9,$B$2,FALSE)</f>
+        <v>0.60322185253885463</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <f>_xll.acq_binomtest(E10,F10,$B$2,TRUE)</f>
+        <v>0.16818032970623617</v>
+      </c>
+      <c r="H10">
+        <f>_xll.acq_binomtest(E10,F10,$B$2,FALSE)</f>
+        <v>0.68732623026634165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <f>_xll.acq_binomtest(E11,F11,$B$2,TRUE)</f>
+        <v>0.236593090512564</v>
+      </c>
+      <c r="H11">
+        <f>_xll.acq_binomtest(E11,F11,$B$2,FALSE)</f>
+        <v>0.76340690948743595</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <f>_xll.acq_binomtest(E12,F12,$B$2,TRUE)</f>
+        <v>0.31267376973365829</v>
+      </c>
+      <c r="H12">
+        <f>_xll.acq_binomtest(E12,F12,$B$2,FALSE)</f>
+        <v>0.8318196702937638</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <f>_xll.acq_binomtest(E13,F13,$B$2,TRUE)</f>
+        <v>0.39677814746114531</v>
+      </c>
+      <c r="H13">
+        <f>_xll.acq_binomtest(E13,F13,$B$2,FALSE)</f>
+        <v>0.89220873259369882</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <f>_xll.acq_binomtest(E14,F14,$B$2,TRUE)</f>
+        <v>0.49016247153664178</v>
+      </c>
+      <c r="H14">
+        <f>_xll.acq_binomtest(E14,F14,$B$2,FALSE)</f>
+        <v>0.94331784854562473</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <f>_xll.acq_binomtest(E15,F15,$B$2,TRUE)</f>
+        <v>0.59584997320476163</v>
+      </c>
+      <c r="H15">
+        <f>_xll.acq_binomtest(E15,F15,$B$2,FALSE)</f>
+        <v>0.98212378690492708</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16">
+        <f>_xll.acq_binomtest(E16,F16,$B$2,TRUE)</f>
+        <v>0.72246720013711063</v>
+      </c>
+      <c r="H16">
+        <f>_xll.acq_binomtest(E16,F16,$B$2,FALSE)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8">
+      <c r="E17">
+        <v>11</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="G17" t="e">
+        <f>_xll.acq_binomtest(E17,F17,$B$2,TRUE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H17" t="e">
+        <f>_xll.acq_binomtest(E17,F17,$B$2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8">
+      <c r="E18">
+        <v>99</v>
+      </c>
+      <c r="F18">
+        <v>100</v>
+      </c>
+      <c r="G18">
+        <f>_xll.acq_binomtest(E18,F18,$B$2,TRUE)</f>
+        <v>0.94551380382129468</v>
+      </c>
+      <c r="H18">
+        <f>_xll.acq_binomtest(E18,F18,$B$2,FALSE)</f>
+        <v>0.99823256793585935</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>100</v>
+      </c>
+      <c r="G19">
+        <f>_xll.acq_binomtest(E19,F19,$B$2,TRUE)</f>
+        <v>1.7674320641406526E-3</v>
+      </c>
+      <c r="H19">
+        <f>_xll.acq_binomtest(E19,F19,$B$2,FALSE)</f>
+        <v>5.4486196178705315E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30B9D5F-797C-49CC-9435-B3BF433B0ECB}">
+  <dimension ref="B1:O18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" ht="15.75" thickBot="1">
+      <c r="C1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15">
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="6">
+        <f ca="1">_xll.acq_min(H2:L18)</f>
+        <v>-0.92800000000000005</v>
+      </c>
+      <c r="D2" s="6">
+        <f t="array" aca="1" ref="D2" ca="1">MIN(IF(ISNUMBER(H2:L18), H2:L18))</f>
+        <v>-0.92800000000000005</v>
+      </c>
+      <c r="E2">
+        <f ca="1">C2-D2</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <f ca="1">RANDBETWEEN(-1000,1000)/1000</f>
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="I2" s="5">
+        <f t="shared" ref="I2:L18" ca="1" si="0">RANDBETWEEN(-1000,1000)/1000</f>
+        <v>0.7</v>
+      </c>
+      <c r="J2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="K2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.57699999999999996</v>
+      </c>
+      <c r="L2" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="6">
+        <f ca="1">_xll.acq_absmin(H2:L18)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D3" s="6">
+        <f t="array" aca="1" ref="D3" ca="1">MIN(ABS(IF(ISNUMBER(H2:L18), H2:L18)))</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" ca="1" si="1">C3-D3</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H3" s="5">
+        <f t="shared" ref="H3:H18" ca="1" si="2">RANDBETWEEN(-1000,1000)/1000</f>
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.08</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.57799999999999996</v>
+      </c>
+      <c r="K3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="L3" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="O3">
+        <f>17*5</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="6">
+        <f ca="1">_xll.acq_max(H2:L18)</f>
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="array" aca="1" ref="D4" ca="1">MAX(IF(ISNUMBER(H2:L18), H2:L18))</f>
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.51400000000000001</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.54700000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="6">
+        <f ca="1">_xll.acq_absmax(H2:L18)</f>
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="array" aca="1" ref="D5" ca="1">MAX(ABS(IF(ISNUMBER(H2:L18), H2:L18)))</f>
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="K5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.65800000000000003</v>
+      </c>
+      <c r="L5" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.245</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15">
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="6">
+        <f ca="1">_xll.acq_sum(H2:L18)</f>
+        <v>4.4000000000000233E-2</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="array" aca="1" ref="D6" ca="1">SUM(IF(ISNUMBER(H2:L18), H2:L18))</f>
+        <v>4.3999999999999789E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.4408920985006262E-16</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.35899999999999999</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.19800000000000001</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.56899999999999995</v>
+      </c>
+      <c r="L6" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.749</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="6">
+        <f ca="1">_xll.acq_count_unique(H2:L18, TRUE)</f>
+        <v>80</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="array" aca="1" ref="D7" ca="1">COUNT(H2:L18)</f>
+        <v>78</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>-6.4000000000000001E-2</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.36899999999999999</v>
+      </c>
+      <c r="K7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="L7" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="6">
+        <f ca="1">_xll.acq_mean(H2:L18)</f>
+        <v>5.6410256410256709E-4</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="array" aca="1" ref="D8" ca="1">AVERAGE(IF(ISNUMBER(H2:L18), H2:L18))</f>
+        <v>5.6410256410256135E-4</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.7462715141731735E-18</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.68799999999999994</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.182</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.28899999999999998</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-7.1999999999999995E-2</v>
+      </c>
+      <c r="L8" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="6">
+        <f ca="1">_xll.acq_stdev(H2:L18)</f>
+        <v>0.51218527465923458</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="array" aca="1" ref="D9" ca="1">_xlfn.STDEV.S(IF(ISNUMBER(H2:L18), H2:L18))</f>
+        <v>0.51218527465923458</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.88500000000000001</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="L9" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.29899999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="6">
+        <f ca="1">_xll.acq_sumofsquares(H2:L18)</f>
+        <v>20.199723999999993</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="array" aca="1" ref="D10" ca="1">SUM(IF(ISNUMBER(H2:L18), H2:L18^2))</f>
+        <v>20.199723999999993</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.57599999999999996</v>
+      </c>
+      <c r="J10" s="5" t="e">
+        <f>1/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="L10" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.28399999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15">
+      <c r="H11" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.22500000000000001</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.11600000000000001</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.56200000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="H12" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.498</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.46700000000000003</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.374</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="H13" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.13800000000000001</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.151</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.92800000000000005</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.17699999999999999</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.13200000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="H14" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.313</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="L14" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.71899999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="H15" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.34599999999999997</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.38100000000000001</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.74299999999999999</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.13</v>
+      </c>
+      <c r="L15" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.40799999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15">
+      <c r="H16" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.04</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.64900000000000002</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="L16" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="8:12">
+      <c r="H17" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.39200000000000002</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.375</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="L17" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12">
+      <c r="H18" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.114</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.82699999999999996</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.75700000000000001</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.92600000000000005</v>
+      </c>
+      <c r="L18" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>-9.6000000000000002E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>